<commit_message>
ticket #9282 cal sheets updated/added to repo for CP05MOAS gliders 388, 389 for multiple deployments.
</commit_message>
<xml_diff>
--- a/CP05MOAS-GL388/Omaha_Cal_Info_CP05MOAS-GL388_00001.xlsx
+++ b/CP05MOAS-GL388/Omaha_Cal_Info_CP05MOAS-GL388_00001.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gauls\Documents\Project Info\WHOI\Marine Integration - OOI\OOInet Migration\Integration\Cal and Ingest Sheets\Repaired GIT\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25823"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14040" windowHeight="6576" tabRatio="377"/>
+    <workbookView xWindow="4240" yWindow="3620" windowWidth="23040" windowHeight="9240" tabRatio="377"/>
   </bookViews>
   <sheets>
     <sheet name="Moorings" sheetId="2" r:id="rId1"/>
@@ -35,7 +30,12 @@
     <definedName name="_FilterDatabase_1_1_1">Moorings!$A$1:$J$73</definedName>
     <definedName name="_FilterDatabase_2">Asset_Cal_Info!$A$1:$F$360</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -78,9 +78,6 @@
     <t>KN-222</t>
   </si>
   <si>
-    <t>SS-2</t>
-  </si>
-  <si>
     <t>Mooring Serial Number</t>
   </si>
   <si>
@@ -138,17 +135,30 @@
     <t>CP05MOAS-GL388-00-ENG000000</t>
   </si>
   <si>
-    <t>39° 49.782' N</t>
-  </si>
-  <si>
-    <t>70° 35.004' W</t>
+    <t>39° 50' N</t>
+  </si>
+  <si>
+    <t>70° 42.5' W</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">SS-2 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>Line</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -211,8 +221,13 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -227,18 +242,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFDEADA"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
         <bgColor rgb="FFBFBFBF"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -300,12 +309,25 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -319,13 +341,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="15" fontId="2" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="20" fontId="2" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="3" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -343,7 +359,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -352,7 +368,7 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -367,6 +383,18 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="15" fontId="9" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="9" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -497,7 +525,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -532,7 +560,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -743,25 +771,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="37.88671875"/>
-    <col min="2" max="2" width="39.44140625"/>
-    <col min="3" max="3" width="14.44140625"/>
-    <col min="4" max="4" width="24.109375"/>
-    <col min="5" max="6" width="17.44140625"/>
-    <col min="7" max="8" width="18.6640625"/>
-    <col min="9" max="9" width="17.88671875"/>
-    <col min="10" max="10" width="12.6640625"/>
-    <col min="11" max="11" width="51.6640625"/>
-    <col min="12" max="1025" width="8.6640625"/>
+    <col min="1" max="1" width="19" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" customWidth="1"/>
+    <col min="3" max="3" width="14.83203125" customWidth="1"/>
+    <col min="4" max="8" width="17" customWidth="1"/>
+    <col min="9" max="11" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" ht="30">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -796,9 +819,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" s="6" customFormat="1" ht="15">
       <c r="A2" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B2" s="4">
         <v>388</v>
@@ -806,42 +829,47 @@
       <c r="C2" s="4">
         <v>1</v>
       </c>
-      <c r="D2" s="5">
-        <v>41918</v>
-      </c>
-      <c r="E2" s="6">
+      <c r="D2" s="24">
+        <v>41917</v>
+      </c>
+      <c r="E2" s="5">
         <v>0.843055555555556</v>
       </c>
-      <c r="F2" s="7">
-        <v>42016</v>
-      </c>
-      <c r="G2" s="4" t="s">
+      <c r="F2" s="25">
+        <v>41986</v>
+      </c>
+      <c r="G2" s="26" t="s">
+        <v>31</v>
+      </c>
+      <c r="H2" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="H2" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="I2" s="4">
-        <v>0</v>
+      <c r="I2" s="27">
+        <v>1000</v>
       </c>
       <c r="J2" s="4" t="s">
         <v>11</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="L2" s="25">
+        <v>33</v>
+      </c>
+      <c r="L2" s="23">
         <f>((LEFT(G2,(FIND("°",G2,1)-1)))+(MID(G2,(FIND("°",G2,1)+1),(FIND("'",G2,1))-(FIND("°",G2,1)+1))/60))*(IF(RIGHT(G2,1)="N",1,-1))</f>
-        <v>39.829700000000003</v>
-      </c>
-      <c r="M2" s="25">
+        <v>39.833333333333336</v>
+      </c>
+      <c r="M2" s="23">
         <f>((LEFT(H2,(FIND("°",H2,1)-1)))+(MID(H2,(FIND("°",H2,1)+1),(FIND("'",H2,1))-(FIND("°",H2,1)+1))/60))*(IF(RIGHT(H2,1)="E",1,-1))</f>
-        <v>-70.583399999999997</v>
+        <v>-70.708333333333329</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -849,419 +877,420 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P18"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="34.5546875"/>
-    <col min="2" max="2" width="25"/>
-    <col min="3" max="3" width="26.109375"/>
-    <col min="4" max="4" width="26.88671875"/>
-    <col min="5" max="6" width="28.88671875"/>
-    <col min="7" max="7" width="11.88671875"/>
-    <col min="8" max="8" width="14.44140625"/>
-    <col min="9" max="9" width="13.44140625"/>
-    <col min="10" max="1025" width="8.6640625"/>
+    <col min="1" max="1" width="28.5" customWidth="1"/>
+    <col min="2" max="2" width="10.1640625" customWidth="1"/>
+    <col min="3" max="3" width="13.5" customWidth="1"/>
+    <col min="4" max="4" width="18.83203125" customWidth="1"/>
+    <col min="5" max="6" width="34.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" ht="45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="F1" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="F1" s="10" t="s">
+    </row>
+    <row r="2" spans="1:16">
+      <c r="A2" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="10">
+        <v>388</v>
+      </c>
+      <c r="C2" s="10">
+        <v>1</v>
+      </c>
+      <c r="D2" s="11">
+        <v>654584</v>
+      </c>
+      <c r="E2" s="12" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A2" s="11" t="s">
+      <c r="F2" s="13">
+        <v>0.61</v>
+      </c>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
+      <c r="I2" s="14"/>
+      <c r="J2" s="14"/>
+      <c r="K2" s="14"/>
+      <c r="L2" s="14"/>
+      <c r="M2" s="14"/>
+      <c r="N2" s="14"/>
+      <c r="O2" s="14"/>
+      <c r="P2" s="14"/>
+    </row>
+    <row r="3" spans="1:16">
+      <c r="A3" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="10">
+        <v>388</v>
+      </c>
+      <c r="C3" s="10">
+        <v>1</v>
+      </c>
+      <c r="D3" s="11">
+        <v>654584</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="13">
+        <v>0.61</v>
+      </c>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="14"/>
+      <c r="J3" s="14"/>
+      <c r="K3" s="14"/>
+      <c r="L3" s="14"/>
+      <c r="M3" s="14"/>
+      <c r="N3" s="14"/>
+      <c r="O3" s="14"/>
+      <c r="P3" s="14"/>
+    </row>
+    <row r="4" spans="1:16">
+      <c r="A4" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="10">
+        <v>388</v>
+      </c>
+      <c r="C4" s="10">
+        <v>1</v>
+      </c>
+      <c r="D4" s="11">
+        <v>654584</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="13">
+        <v>0.61</v>
+      </c>
+      <c r="G4" s="14"/>
+      <c r="H4" s="14"/>
+      <c r="I4" s="14"/>
+      <c r="J4" s="14"/>
+      <c r="K4" s="14"/>
+      <c r="L4" s="14"/>
+      <c r="M4" s="14"/>
+      <c r="N4" s="14"/>
+      <c r="O4" s="14"/>
+      <c r="P4" s="14"/>
+    </row>
+    <row r="5" spans="1:16">
+      <c r="A5" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="10">
+        <v>388</v>
+      </c>
+      <c r="C5" s="10">
+        <v>1</v>
+      </c>
+      <c r="D5" s="11">
+        <v>654584</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" s="13">
+        <v>0.61</v>
+      </c>
+      <c r="G5" s="14"/>
+      <c r="H5" s="14"/>
+      <c r="I5" s="14"/>
+      <c r="J5" s="14"/>
+      <c r="K5" s="14"/>
+      <c r="L5" s="14"/>
+      <c r="M5" s="14"/>
+      <c r="N5" s="14"/>
+      <c r="O5" s="14"/>
+      <c r="P5" s="14"/>
+    </row>
+    <row r="6" spans="1:16">
+      <c r="A6" s="15"/>
+      <c r="B6" s="10"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="16"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="14"/>
+      <c r="I6" s="14"/>
+      <c r="J6" s="14"/>
+      <c r="K6" s="14"/>
+      <c r="L6" s="14"/>
+      <c r="M6" s="14"/>
+      <c r="N6" s="14"/>
+      <c r="O6" s="14"/>
+      <c r="P6" s="14"/>
+    </row>
+    <row r="7" spans="1:16" s="20" customFormat="1">
+      <c r="A7" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="B2" s="12">
-        <v>388</v>
-      </c>
-      <c r="C2" s="12">
-        <v>1</v>
-      </c>
-      <c r="D2" s="13">
-        <v>654584</v>
-      </c>
-      <c r="E2" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="F2" s="15">
-        <v>0.61</v>
-      </c>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
-      <c r="I2" s="16"/>
-      <c r="J2" s="16"/>
-      <c r="K2" s="16"/>
-      <c r="L2" s="16"/>
-      <c r="M2" s="16"/>
-      <c r="N2" s="16"/>
-      <c r="O2" s="16"/>
-      <c r="P2" s="16"/>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A3" s="17" t="s">
+      <c r="B7" s="10">
+        <v>388</v>
+      </c>
+      <c r="C7" s="10">
+        <v>1</v>
+      </c>
+      <c r="D7" s="11">
+        <v>3206</v>
+      </c>
+      <c r="E7" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="F7" s="18">
+        <v>124</v>
+      </c>
+      <c r="G7" s="19"/>
+      <c r="H7" s="19"/>
+      <c r="I7" s="19"/>
+      <c r="J7" s="19"/>
+      <c r="K7" s="19"/>
+    </row>
+    <row r="8" spans="1:16" s="20" customFormat="1">
+      <c r="A8" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="B3" s="12">
-        <v>388</v>
-      </c>
-      <c r="C3" s="12">
-        <v>1</v>
-      </c>
-      <c r="D3" s="13">
-        <v>654584</v>
-      </c>
-      <c r="E3" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="F3" s="15">
-        <v>0.61</v>
-      </c>
-      <c r="G3" s="16"/>
-      <c r="H3" s="16"/>
-      <c r="I3" s="16"/>
-      <c r="J3" s="16"/>
-      <c r="K3" s="16"/>
-      <c r="L3" s="16"/>
-      <c r="M3" s="16"/>
-      <c r="N3" s="16"/>
-      <c r="O3" s="16"/>
-      <c r="P3" s="16"/>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A4" s="17" t="s">
+      <c r="B8" s="10">
+        <v>388</v>
+      </c>
+      <c r="C8" s="10">
+        <v>1</v>
+      </c>
+      <c r="D8" s="11">
+        <v>3206</v>
+      </c>
+      <c r="E8" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="F8" s="18">
+        <v>700</v>
+      </c>
+      <c r="G8" s="19"/>
+      <c r="H8" s="19"/>
+      <c r="I8" s="19"/>
+      <c r="J8" s="19"/>
+      <c r="K8" s="19"/>
+    </row>
+    <row r="9" spans="1:16" s="20" customFormat="1">
+      <c r="A9" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="B4" s="12">
-        <v>388</v>
-      </c>
-      <c r="C4" s="12">
-        <v>1</v>
-      </c>
-      <c r="D4" s="13">
-        <v>654584</v>
-      </c>
-      <c r="E4" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="F4" s="15">
-        <v>0.61</v>
-      </c>
-      <c r="G4" s="16"/>
-      <c r="H4" s="16"/>
-      <c r="I4" s="16"/>
-      <c r="J4" s="16"/>
-      <c r="K4" s="16"/>
-      <c r="L4" s="16"/>
-      <c r="M4" s="16"/>
-      <c r="N4" s="16"/>
-      <c r="O4" s="16"/>
-      <c r="P4" s="16"/>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A5" s="17" t="s">
+      <c r="B9" s="10">
+        <v>388</v>
+      </c>
+      <c r="C9" s="10">
+        <v>1</v>
+      </c>
+      <c r="D9" s="11">
+        <v>3206</v>
+      </c>
+      <c r="E9" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="F9" s="18">
+        <v>1.0760000000000001</v>
+      </c>
+      <c r="G9" s="19"/>
+      <c r="H9" s="19"/>
+      <c r="I9" s="19"/>
+      <c r="J9" s="19"/>
+      <c r="K9" s="19"/>
+    </row>
+    <row r="10" spans="1:16" s="20" customFormat="1">
+      <c r="A10" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="B5" s="12">
-        <v>388</v>
-      </c>
-      <c r="C5" s="12">
-        <v>1</v>
-      </c>
-      <c r="D5" s="13">
-        <v>654584</v>
-      </c>
-      <c r="E5" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="F5" s="15">
-        <v>0.61</v>
-      </c>
-      <c r="G5" s="16"/>
-      <c r="H5" s="16"/>
-      <c r="I5" s="16"/>
-      <c r="J5" s="16"/>
-      <c r="K5" s="16"/>
-      <c r="L5" s="16"/>
-      <c r="M5" s="16"/>
-      <c r="N5" s="16"/>
-      <c r="O5" s="16"/>
-      <c r="P5" s="16"/>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A6" s="17"/>
-      <c r="B6" s="12"/>
-      <c r="C6" s="12"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="18"/>
-      <c r="G6" s="16"/>
-      <c r="H6" s="16"/>
-      <c r="I6" s="16"/>
-      <c r="J6" s="16"/>
-      <c r="K6" s="16"/>
-      <c r="L6" s="16"/>
-      <c r="M6" s="16"/>
-      <c r="N6" s="16"/>
-      <c r="O6" s="16"/>
-      <c r="P6" s="16"/>
-    </row>
-    <row r="7" spans="1:16" s="22" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="A7" s="11" t="s">
+      <c r="B10" s="10">
+        <v>388</v>
+      </c>
+      <c r="C10" s="10">
+        <v>1</v>
+      </c>
+      <c r="D10" s="11">
+        <v>3206</v>
+      </c>
+      <c r="E10" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="F10" s="18">
+        <v>3.9E-2</v>
+      </c>
+      <c r="G10" s="19"/>
+      <c r="H10" s="19"/>
+      <c r="I10" s="19"/>
+      <c r="J10" s="19"/>
+      <c r="K10" s="19"/>
+    </row>
+    <row r="11" spans="1:16">
+      <c r="A11" s="15"/>
+      <c r="B11" s="10"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="21"/>
+      <c r="G11" s="19"/>
+      <c r="H11" s="19"/>
+      <c r="I11" s="19"/>
+      <c r="J11" s="19"/>
+      <c r="K11" s="19"/>
+    </row>
+    <row r="12" spans="1:16">
+      <c r="A12" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="12">
-        <v>388</v>
-      </c>
-      <c r="C7" s="12">
-        <v>1</v>
-      </c>
-      <c r="D7" s="13">
-        <v>3206</v>
-      </c>
-      <c r="E7" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="F7" s="20">
-        <v>124</v>
-      </c>
-      <c r="G7" s="21"/>
-      <c r="H7" s="21"/>
-      <c r="I7" s="21"/>
-      <c r="J7" s="21"/>
-      <c r="K7" s="21"/>
-    </row>
-    <row r="8" spans="1:16" s="22" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="A8" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="B8" s="12">
-        <v>388</v>
-      </c>
-      <c r="C8" s="12">
-        <v>1</v>
-      </c>
-      <c r="D8" s="13">
-        <v>3206</v>
-      </c>
-      <c r="E8" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="F8" s="20">
-        <v>700</v>
-      </c>
-      <c r="G8" s="21"/>
-      <c r="H8" s="21"/>
-      <c r="I8" s="21"/>
-      <c r="J8" s="21"/>
-      <c r="K8" s="21"/>
-    </row>
-    <row r="9" spans="1:16" s="22" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="A9" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="B9" s="12">
-        <v>388</v>
-      </c>
-      <c r="C9" s="12">
-        <v>1</v>
-      </c>
-      <c r="D9" s="13">
-        <v>3206</v>
-      </c>
-      <c r="E9" s="19" t="s">
-        <v>23</v>
-      </c>
-      <c r="F9" s="20">
-        <v>1.0760000000000001</v>
-      </c>
-      <c r="G9" s="21"/>
-      <c r="H9" s="21"/>
-      <c r="I9" s="21"/>
-      <c r="J9" s="21"/>
-      <c r="K9" s="21"/>
-    </row>
-    <row r="10" spans="1:16" s="22" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="A10" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="B10" s="12">
-        <v>388</v>
-      </c>
-      <c r="C10" s="12">
-        <v>1</v>
-      </c>
-      <c r="D10" s="13">
-        <v>3206</v>
-      </c>
-      <c r="E10" s="19" t="s">
-        <v>24</v>
-      </c>
-      <c r="F10" s="20">
-        <v>3.9E-2</v>
-      </c>
-      <c r="G10" s="21"/>
-      <c r="H10" s="21"/>
-      <c r="I10" s="21"/>
-      <c r="J10" s="21"/>
-      <c r="K10" s="21"/>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A11" s="17"/>
-      <c r="B11" s="12"/>
-      <c r="C11" s="12"/>
-      <c r="D11" s="13"/>
-      <c r="E11" s="19"/>
-      <c r="F11" s="23"/>
-      <c r="G11" s="21"/>
-      <c r="H11" s="21"/>
-      <c r="I11" s="21"/>
-      <c r="J11" s="21"/>
-      <c r="K11" s="21"/>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A12" s="11" t="s">
+      <c r="B12" s="10">
+        <v>388</v>
+      </c>
+      <c r="C12" s="10">
+        <v>1</v>
+      </c>
+      <c r="D12" s="11">
+        <v>9088</v>
+      </c>
+      <c r="E12" s="19"/>
+      <c r="F12" s="22"/>
+      <c r="G12" s="19"/>
+      <c r="H12" s="19"/>
+      <c r="I12" s="19"/>
+      <c r="J12" s="19"/>
+      <c r="K12" s="19"/>
+    </row>
+    <row r="13" spans="1:16">
+      <c r="A13" s="9"/>
+      <c r="B13" s="10"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="19"/>
+      <c r="F13" s="22"/>
+      <c r="G13" s="19"/>
+      <c r="H13" s="19"/>
+      <c r="I13" s="19"/>
+      <c r="J13" s="19"/>
+      <c r="K13" s="19"/>
+    </row>
+    <row r="14" spans="1:16">
+      <c r="A14" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="B12" s="12">
-        <v>388</v>
-      </c>
-      <c r="C12" s="12">
-        <v>1</v>
-      </c>
-      <c r="D12" s="13">
-        <v>9088</v>
-      </c>
-      <c r="E12" s="21"/>
-      <c r="F12" s="24"/>
-      <c r="G12" s="21"/>
-      <c r="H12" s="21"/>
-      <c r="I12" s="21"/>
-      <c r="J12" s="21"/>
-      <c r="K12" s="21"/>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A13" s="11"/>
-      <c r="B13" s="12"/>
-      <c r="C13" s="12"/>
-      <c r="D13" s="13"/>
-      <c r="E13" s="21"/>
-      <c r="F13" s="24"/>
-      <c r="G13" s="21"/>
-      <c r="H13" s="21"/>
-      <c r="I13" s="21"/>
-      <c r="J13" s="21"/>
-      <c r="K13" s="21"/>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A14" s="11" t="s">
+      <c r="B14" s="10">
+        <v>388</v>
+      </c>
+      <c r="C14" s="10">
+        <v>1</v>
+      </c>
+      <c r="D14" s="11">
+        <v>192</v>
+      </c>
+      <c r="E14" s="19"/>
+      <c r="F14" s="22"/>
+      <c r="G14" s="19"/>
+      <c r="H14" s="19"/>
+      <c r="I14" s="19"/>
+      <c r="J14" s="19"/>
+      <c r="K14" s="19"/>
+    </row>
+    <row r="15" spans="1:16">
+      <c r="A15" s="9"/>
+      <c r="B15" s="10"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="19"/>
+      <c r="F15" s="22"/>
+      <c r="G15" s="19"/>
+      <c r="H15" s="19"/>
+      <c r="I15" s="19"/>
+      <c r="J15" s="19"/>
+      <c r="K15" s="19"/>
+    </row>
+    <row r="16" spans="1:16">
+      <c r="A16" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="B14" s="12">
-        <v>388</v>
-      </c>
-      <c r="C14" s="12">
-        <v>1</v>
-      </c>
-      <c r="D14" s="13">
-        <v>192</v>
-      </c>
-      <c r="E14" s="21"/>
-      <c r="F14" s="24"/>
-      <c r="G14" s="21"/>
-      <c r="H14" s="21"/>
-      <c r="I14" s="21"/>
-      <c r="J14" s="21"/>
-      <c r="K14" s="21"/>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A15" s="11"/>
-      <c r="B15" s="12"/>
-      <c r="C15" s="12"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="21"/>
-      <c r="F15" s="24"/>
-      <c r="G15" s="21"/>
-      <c r="H15" s="21"/>
-      <c r="I15" s="21"/>
-      <c r="J15" s="21"/>
-      <c r="K15" s="21"/>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A16" s="11" t="s">
+      <c r="B16" s="10">
+        <v>388</v>
+      </c>
+      <c r="C16" s="10">
+        <v>1</v>
+      </c>
+      <c r="D16" s="11">
+        <v>50166</v>
+      </c>
+      <c r="E16" s="19"/>
+      <c r="F16" s="22"/>
+      <c r="G16" s="19"/>
+      <c r="H16" s="19"/>
+      <c r="I16" s="19"/>
+      <c r="J16" s="19"/>
+      <c r="K16" s="19"/>
+    </row>
+    <row r="17" spans="1:11">
+      <c r="A17" s="9"/>
+      <c r="B17" s="10"/>
+      <c r="C17" s="10"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="19"/>
+      <c r="F17" s="22"/>
+      <c r="G17" s="19"/>
+      <c r="H17" s="19"/>
+      <c r="I17" s="19"/>
+      <c r="J17" s="19"/>
+      <c r="K17" s="19"/>
+    </row>
+    <row r="18" spans="1:11">
+      <c r="A18" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="B16" s="12">
-        <v>388</v>
-      </c>
-      <c r="C16" s="12">
-        <v>1</v>
-      </c>
-      <c r="D16" s="13">
-        <v>50166</v>
-      </c>
-      <c r="E16" s="21"/>
-      <c r="F16" s="24"/>
-      <c r="G16" s="21"/>
-      <c r="H16" s="21"/>
-      <c r="I16" s="21"/>
-      <c r="J16" s="21"/>
-      <c r="K16" s="21"/>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A17" s="11"/>
-      <c r="B17" s="12"/>
-      <c r="C17" s="12"/>
-      <c r="D17" s="13"/>
-      <c r="E17" s="21"/>
-      <c r="F17" s="24"/>
-      <c r="G17" s="21"/>
-      <c r="H17" s="21"/>
-      <c r="I17" s="21"/>
-      <c r="J17" s="21"/>
-      <c r="K17" s="21"/>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A18" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="B18" s="12">
-        <v>388</v>
-      </c>
-      <c r="C18" s="12">
-        <v>1</v>
-      </c>
-      <c r="D18" s="13">
-        <v>388</v>
-      </c>
-      <c r="E18" s="21"/>
-      <c r="F18" s="24"/>
-      <c r="G18" s="21"/>
-      <c r="H18" s="21"/>
-      <c r="I18" s="21"/>
-      <c r="J18" s="21"/>
-      <c r="K18" s="21"/>
+      <c r="B18" s="10">
+        <v>388</v>
+      </c>
+      <c r="C18" s="10">
+        <v>1</v>
+      </c>
+      <c r="D18" s="11">
+        <v>388</v>
+      </c>
+      <c r="E18" s="19"/>
+      <c r="F18" s="22"/>
+      <c r="G18" s="19"/>
+      <c r="H18" s="19"/>
+      <c r="I18" s="19"/>
+      <c r="J18" s="19"/>
+      <c r="K18" s="19"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>